<commit_message>
update excel, fix card
</commit_message>
<xml_diff>
--- a/Book3.xlsx
+++ b/Book3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="8750" windowHeight="6800"/>
+    <workbookView windowWidth="18530" windowHeight="6950"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,18 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
-  <si>
-    <t>id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>name</t>
   </si>
   <si>
+    <t>username</t>
+  </si>
+  <si>
     <t>email</t>
   </si>
   <si>
-    <t xml:space="preserve">phone </t>
+    <t>phone</t>
   </si>
   <si>
     <t>company</t>
@@ -52,37 +52,43 @@
     <t>web</t>
   </si>
   <si>
-    <t>dat</t>
+    <t>dat.lethanh2</t>
+  </si>
+  <si>
+    <t>Lê Thành Đạt</t>
   </si>
   <si>
     <t>dat.lethanh2@ncc.asia</t>
   </si>
   <si>
-    <t>ncc</t>
+    <t>NCCPLUS VIETNAM JSC</t>
   </si>
   <si>
     <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAoHCBYWFRgVFRUYGBgYGBoYGhwYGBgYGBgYGBgcGhoaGhkcIS4lHB4rHxoYJjgmKy8xNTU1GiQ7QDs0Py40NTEBDAwMEA8QHhISHjQhJCs0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0NDQ0ND80NDQ0ND03NP/AABEIARoAswMBIgACEQEDEQH/xAAcAAAABwEBAAAAAAAAAAAAAAAAAQMEBQYHAgj/xABFEAACAQIDBAYGBwcCBgMBAAABAgADEQQSIQUxQVEGImFxgZETMqGxwdEHQlJUYpPwFSNygpKy4RTxJENzosLSNFNjF//EABkBAAMBAQEAAAAAAAAAAAAAAAABAwIEBf/EACERAAICAgIDAQEBAAAAAAAAAAABAhESIQMxQVFhIgRx/9oADAMBAAIRAxEAPwDSLQQ7QWnacNB2hEwi0a4raCILu6oPxMB74DHQIgtIB+k2G3+lHeA59qi3tjyhtlCAxPVO5wLr48jAeLJO0EbVNooNcykaagi2sdExWJxCnVoQhiMVB5YMs6EEVjoICCHBAAQQrQWgB1aFaAQzADmC0MCACABWgtOoUACghwQAMRPU7twNu02hZpCbWL1H/wBMhKhhndwfUQWBRfxMdO4seEVDjsSxO1alZ2pYQDqnLUrMAUS2hCD67du4RGn0fpoc1V3qvvuxLN4HePC0nEpJSRUpqFA0Ue8mQW29uLRVgozuLZydFUndmI3t+EeyC9sovUTnHVsLQHWooSeaKxP8x3SsYrbiI96CJTz6MEvZuV1KhfG19eMgtq7Zao13fuG4eQkHiMbY3Jvrffuicr6KKNdkvi8SzPqbgcBpru8NJcsB02yIq1EzsqhQVIG4WuQd57ZmuGqs9zz47rR0lJgb3v3RW0NxUjS8N06uwDUbAm3Ve7eAI+MtuDxqVBdDe28biD2iYajsDe9v1xkvsrbD0HDqe8G+Vhya0FL2ZlxJ9Gyi86UyC2H0lpYiyk5Kh+qTo38Dce7fJ0LNWmQcWtMO0ICdWgAgIFoRigEGWZsdCdoAsUyzoLHYUJWgtFgsPJM2axG8EX9HDFOPJCxY3tBHHo4IZDxI2p1deHH5iROyF6r1m0NV3YknQJTPo015ZVzfzmTVVLggb7GQGy6d6NFN3Uu455LAjxbfzsZsxHoX2jimRC49dyqUwR6uY6Ejuux7rTLOkG0QWyKTkS9tfWJ1ZyeJJ4y69Ltom4UfV0/nYdbyW3nMux5LOR+u2Zbt0X41SsbPVZt2nhGhQlo9Y2BA4e+CjR4wWjUtiNB29VR3x1Y8z5yY2fsFqhBAsDLBS6KAf7TMpI1GLKYlY3s1wefuvHeGqZgQdCN/wPdLJiuizW0PskK2znpMC43aX3gqfqt2TFm8TnDYkobHgd3FTzXlNS6J9IhVUU6j3f6rHTP2H8XvmW4mmL2P8rfBu33wYXFNSYHUa6jkRFflGZRT0ze7QESv9FdvCugVj1wL/wAY5944ywyidnPKNBqZ1eJQXjozYrDESDw1eKh5Cl4Lws0EVDyDDTsGJwCFDTFLwTmCILGlpXqdX0depSUZmc5qY+qLgu6k/VszM1uNzbdJv/Sqd+Y/ztbyvIza1FBh6thly5nUr1SrjcykbjKGI0UDpHiAXexuqMwv9pvrN4m/gBKjUW2Z+NreOv68JM4026nIC/aT+jI3EqNF5an4CSUt2deNKiOenw7vM/oSb2Ls/Ow9siwMzheep8f8S8dHMOB5wlKhxjZY9m4UKoAEkQgidLdFxMobEXpyJ24aaJmcXJ0UcWPISbdrC8qNeoWqnEVdES4pqf7j7/8AaAEPW2JVyF2CqDuTW4Hed3dIhhk0YZk3fiTsN+ElsZtGtiMxptkANluDdyCBYAbvWB14X3Wjw7AfJmJu9ute1m5g/ODtAqZG7Gxb0XDI2l7qeTcj37u2a7sraArU1deI1H2W4iYoEai2t8hNtd6nirS69DtolHyFuq9u49vePdHGSTJzhaNEDQjCUTqWOXYVoIcK0YgXh3gtCiA7DzoPEwIcVDsUzQROCFDs5WQ/SAgUKl9xB/uA+UmJWem+Iy4YrxdwPC1z8I3pBBfpGZYl7kueZI9w+PnIirXvc8BoO1jaPMa2thykcBmGm4MB7RII7WxfAG9fxPs0l+2EOHaZm6Vcla/4j7TL9s/FhEaodbC4A4k2AHmZmXaNQemXFLAXJsO2N12xRLZFdWPYb+0SAbZb1V9Ji6jAHUU1NgvK/b3axqmIpI5SgmYjflIuLAnVmIF9DpfgY/8ADP8ApdFOaQu19mF7AW0YEgi4IG8W4xbZddioazC/BrXHkTJYDNrBb7Dor+A2VkOYjXt1sOQ5CTFOjFqgsIitYRt0OKsh9sbLUtqLhwQRzZRcHvyg6/hEq+ymKO1Ik9RxlbiNdCPMec0Gogcp2Mf7GHxlH2nhCmJJH2CfFWI+Akm0UUTU9nYosi5tGsCeR03jsj4GRmzVDUk5gbxvBEdq5GjefA/rlOqP6imefNYyaHJEK0JTAYzIZEK0EMGABWgtOrwQsDi0E7ghYqGmKxCoOsbk+qo9Zrb7D3k6DeSJmvSvaLVHIYjq2AVSSEuQdTxY6HhoBJfHY+rXqGhhVZybekrNa2hOp4WHBBoORlf6UYJaDiihLZVVmZvWd31LMfhMN6Lwikys4vQFuYAHiB/mMMIPW7GU++8fbR9YDgov47oyw7WD9pt5D/MyuizGGJPXPafjLv0VxCuiZtSjA+K7r+wykYsda/f7DHnR/aRpVbn1SQG+cUo2hRlTNE6SLXfKtIEm+pvawO899r275xs/YIVswTKNLLcG3e1gTx33375Y8BUV0DCxuI/FMRRbRRpPsbUKOUWnSPbuilQ6RjUpB1ynUE6jgew8xCWgSsemtmsFtv1vxHZOsStMKWc2AF9N+nIDUmQOM2ilLQbxppuB5dp7I52GxqOGe5JPVU7+1m8Nw7ZNs6eP+dtZdIkNjUnzddcuYXA35ewnnaQW3Eti3W31NO9ut85oKICbyv7WwAfEZvsp4kliR4ayUuhRach7sV7p3E+R6ynyMkyAZE7NORlB0DKUsftU2I9oI8pLhbTp/nl+a9HD/VGpWvJwlxp5f5iwnBInay7OWgWh5YIZgMK0EEEADgggiAY4DAJRQIg72OrO3FmPEkzLullfPi3PBTb+kZB7QTNZrvlUnkL+WsxrbJOck72VT45R+vGZl0V49u2V3H1bXPaT4DQRrS0KryUk97G/yhYx8zWHE+wbpzSbrk9tvKZ8FvI3xQ184MHYnKfCd4odaIU13zS6E+y/9F9rvTGRw2QcSPV8eI90vtLEBgCDcGYzsLba0gVqhjrcFQD4HXf2yT2d03ZKhzJ+5J0UeunaOBvvI8u2VOyilGjUKjSJr+nN0p5VFtWa5btCqPeTHGzdrUa65qbqw423qeTLvU98e3EyyiaWyv09jspvpf7RJJ8NNJN7KplNw7yd5/xHAUQy9oJIo+eTWJY8GwK3kdj0yYlHPqupp9gbePMA+Ud7Kw7AZnBF9wO+3MjhHdeirgqwuDpy8QeBHA9klPekYTpkXjaNnte2ch0PKootb+ZY+wlbOgbcdxHIjfGVi37itfMNUfdnA3MOTjiPnOMPUdGOYXceuFGlReDoPtDiO+b43izPJHKP0l8s5y23TtHBAINwdxhzqTOBqnTCWHaEYcDILQWhwQAK0EOCAETjWKUnVzcBHIY8QEO/tmU9JKTLSp1SLekDoNb6UStP3CbFjqIZHUi4KMPZM36R7Pb9m4ZjdsjNfd1Q7sP7svnBleNmYFuuOzXxi1NfVP4oilM59efvj16dlX+KZKob41NTGi7++SGPXrHuv7pG1N4guhPsTZdYtTHDyib750pt3RiR0UZDnRmRhxVipHcRrLv0O2/UqKUdyzrxNrsp3HttulQYbx2Rx0YqFcQrDkQe64k5K0Ui6Zq61X5+yL0Wa98xuIjhzcAxyiznpl00W7A4oOo521747AsZXNkV8rWPGWINrFQpfAV8OrizAHiOYPMHge2MsVhWNgbm2qsujqedtx/WkDY61fJwsAe+SjKDNIy7VFdWs6Pbex3qeqlQ80J0R/wm1/bJLDYlHF1O7QgizKeTKdQY5q0wdGAI7d8i2ogVBckHg31gPsvzHI+46mkZUYlBT+MkbQwImjG5Vt48iOY/WkVy+2WUkzmlBphWgtOiphRmaCgggjMiVX1T3GVvFYb0mC9Hxeico/EWDqfAkHwk/j36jAbyCPPfCwlEKiL9lFAv2KBA2tHnmooLq1rai9+HWtOqvqL3n4x50hRUxdZUN1Fapa271gdO4kjwjRtSi95Pde/uiovYntBdb9lvZ/iRL8JMYjrAnt+BkYKJawA5e8xiY3qzuihYW8pP4HYTuwOS/HrKQPE/KWGl0dVSlwMzsDYC1gupsOXCGLoVqykeifNlCm408pYdg7JKkuw1I8uMs77HVHJy2Daj4jz98cGkFFhJyT6Kxrsc4FiFEkqbAxphafVjhVtJY0UTHNNtdJL0dokWuLyJppxEcKsVWOzhqhz5uN7y14WpmUHjaVXJrJXZmJy6Hd7oNA9od4vG26q+tuPZGWFP7xeN7+6HiFAJN+M4wtUZ17/hHGIukSeKSw6ptppyH+IQrCynsMLaL7u6RdfGKlsxCi287gfhfd5Tai1snknol8PiMzHlraJ/6rW0YU6xUEjkbeUapXLanjNyi70Yi15LHmEEhFxJhTOMvZqo+h7iU0txaw7r8u4XPhILpb0mXDUzlF3dT6ME20tbPbeEHM2vwvHm39piihY20GbXVVF7AsONzoFG8jleZNtxXqWr1nI9Ic6o+rumtncjRV3BVHlbfRsjGNkFTBJLnuW/EnUt5zqqcmvEjKOwAanzgRizXt1Ru5E8Jw/XcDhu/Xt84FBVUOTvHwkn0cpEPbJm42tv/V40q2vb9cpbOj+z2TJVPO5/hIsYR7CXRLYdqhWyUCDzcqq+wk+ySOA2cQc7kM5HAWVexeySKpO1E6KOfIb4jBB0ykbjcd/+YwTZqHXXzk2sjcajI2dfVPrDkefcff3yc4+SkJ+AkwYHExzToIN4J8be6cU3uIpeRcSykPcNh6TCwUqexiffFG2aBufzEYI9o4XFNzk3B+Dakg2wzLyMbljFqtc843vNRj7FKXoJnJ3xxs1LuSTYAfr3RAxzTWy256mVjGyUpUjuu9yY0xtEOtiLgix7jF2gI0l1FUQcndjHAVCBkY3scvjw8CNfZBRbS3LSLNR1vzHu1B8Iiu89598lPSKw2KZjBBBI2UK70/xY/wBQlJxemCKrqDq4W6hOwHIRfhnaUPaOKfE1WqVDvO4aCw3ADgoGgHKS/S3HtUrVKnB2K0+AKp1LjsLBz4mQadVO0wbFFaOKrgA23AW8x8veIMBTsC57h/Ef8RBgWbKO8953CPBvVBw/RMLNJDzZWDNSoBwvczRFpgLlA0taQnRzChRmtqfcJPsY4uhNWSOGbMins9o0iltY32Y3VI5N79fnHTb50wdo55KmEIZW+/UGEYFM2YGRo5D+E7uzsMVEcxBqBHq+R+Bk5Q8orCfhnM6E5seIMMSdFLOiZzO1pkxRKYG/WNRbE5I7wmHubncI59EC2m7jEVY7uE7qPawHjNKLRNysPE4XLqDp7pxhtGF/Hukg3WTw+EjEMcW2mmJpJ2hSvQKk8r/7RhXWzH9cJNZ7r4e6Q20XtUA5oD7SPhIzetlYLejiCcwSdlTMOkKsFw6MqKUQIcjq9yXZyzFdASzNpwkZiqgUWG5Rqe3ebST6QVHdC7EAkmyjegB3WHH9b7yuu1wB+I+Nv9odiFcO2RSx37/OO9hjOwPM+yRLuSGHdbw/Rk90SS4HlAZoOzqdlEfERLCrYCLmAUONnaFhzAPl/vHjSOwT9cDncfH4STYS3DK0Q5Y0xO8AghzopkGwCHeFBHQWGIJzBaFDs7zTkvDE5hQrOqTa3ilXfExATFWx2PaFXqgRtUGphIYGmcaY3LQtRfS0iNot++X/AKajyd7+8STpSK2uLVEPNWHkR85HmWi3C9nd4JzeCQLGU7RxStTsiKiqTYgEM17DrEk3+EhXp2APj5yS2lWGTQBQbWA4CIFLoAd4AHyMaBkXVNgCOctPRAC+m695Vqu6x3gyzdBl33+1G+hLs0qiNIs0SoxUxGiOTEFMRTA3O+U9mhlleVmov76j/wBRfZrLMRK8C7I876OCIIZhTqTOcEEEKBkOCckwXjsA4cTdwoLHQAEnuAuZXm6c4Af8/wAqdU+XUiHRZYLxvgcWlVEqIbo4DKbEXB7DqIveAjtDO3Gkgsd0ow1Cr6KtVyPYNqjFbNuuyqQPGTxNxE2aSOUO+R22vWpn+MeeQ/Ax8u490abVS9MNxR1Pger8R5SPKrRTjdMREE4DQTno6jGsYS7hOR62vs9/lEExJ9KbagnL4bvgIAbAkasdB47z+uc5pplI7LsfD/NhNUYOsamVgedx5bpY+hfrHvlertdEvvufZLN0RpEANz+BtF4DyaDS3TtzpEKLaRVzpA0IYNM1dTwW58SCPdeTxMjdlUt78zYR85J0EtxKokOV2zoG8KrUVFLuwVVBZmJsAALkk8BKrsXpgtfGHDqlkCvZ2IzO6EbgNAtg54ndunf0k4xkwLhb/vHSmTyU3Y+YS380oidEhs3pHhsRUalRqZ2Rcx6pCkXAJUkdbUjdzjjbW01w9F6zbkGg4sx0VR3kgTK/o4rBcaoP10qKO/Ln/wDCXv6QKJbA1bfVKN4LUW/sJmr0DSszbE9Mcc5JOIZQeCBUA7AQL+2T/QPpXWNcYes7VFqk5WZizI4BO871IG7gbWhfRfhqbtXD00dlCMpdVawJYNa40+rLJs3oZhqeIFZXdnR84XMgVSSSOqFvlgrG6LWy3Fjx085gm2dlvhqrUalsygG4NwVOqnym93mR/Sen/GHto0z/AHD4RszE0noxg3o4alSfLmRSDlJI1YkakDgRJUmNdn1M1Kmx+siN5oDHIEGIxXp3Wz46tyUqn9KKD7by67T2jUfZOGxFOo6unowzKSDdM1Jr24ZrXvpM42tiPSYis/23dvAubey00z6K8SHwb0m1CVGFt90dQ3lcvMFPA06DdLMRXrmhXKMvo2YNkCvmDKBcrZT6x4S91EzKy/aFvHh7bTLOjdIUa+NWw9LRo1Hpkk2BouCwI3EEhPAaSZ2d9ItMnLiKbUzf1k66acSPWHheJ7CvRaKbGwgidOqtUCpSyuj9ZWFxe+/Q7tbjwgnPgy2aMdp7sx3bhCZeHE7+wcoqlPQG2g3dvznZp8OGpY92/wDXMgRWOhs4vlA4fGX3YOGyIg45VPmLyq7J2c1aslIDrORfsBF79wXWaI9EK5sNOETNIe0t06bdOaZ0jjDJdwPHyjWxPRHbL6T03xT4NFYejVgGOmd0NnAXlvN+NjLCwNjbfY277aTF9q444falSsv1MSzEc1J648VLDxm1U6gYBlNwwBB5gi4PlOlLVHPIxLoNXKY/Dkn1nKn+dGX3sJsO2Nl08TT9FVBKFlY5TlN1Nxrw5eMzTpTTWjtWmUUIA2GcBQFAAKg2A/hM1hppGWzD9hkUNpIvBcSafgztS9zTXtr4P01CrSBAL03QE7gzKcpPYDaY90n/AHWPrsN61zUHiRUHvE2wtyjQSMBxOHrYeo1Js6ODYqpIzDha3rKeE7wGLrYWqKi5kdRezAjMDwZTvUzVE6Y4Rq60utnL+jzFAApuRYuTcLeVD6S6qPiKbI6ufRZHysGylXYi9jobMfKZNWajgqudEcbnRXHcyg/GZj9KtO2Jpt9qio/pdvnL90Pq58Hh2vf90i+KjKfaJl/Tfbf+pr2yZPRF6XrZs2V2624W7o2ZXZqnR574XDnnRp/2LHePr5KVR/sI7f0qT8Jje0elNV6VClTZ6IpUwjZKjDOVAAY5bW3Hnvlkx+3XTZNG/XNcPRdmLFgOuL3vqbC2sLDEoWFxDJmtY50KG4vo2/uOm+Xj6JsVbEVaXB6WbxpsB7nPlIDohVoio6VsOtYMjsuYkFTSR6hAt9oLa/C0HRTaiYfHJWY5KQZw29sqMjBQbamxy+URosHSQegx9drdWrQddP8A9adj/wB4jXbXRhTg6OKoq7u6IaiqMwXMhYvYC6i4A5dbhJr6UaAVqNUfWV0PaBqP7/ZIjYlR0x+CXMwD0aG42DI+HzBTbeAWO/nEwRfuhCBcDhx+C/8AUxb4wSbywTIWYdUuzKiizEKCeCX1Yk89T3BYuyqxFxZABUYbuoATTp9jMoJ73HKHgsIWXFVTqtNPNqtRaXhZWqHxnFXrhFGhquz25JmCUx3AIT/NOc6C7fRpswkPi3HWcOtPu+uw5fZHcZNYlNZOYHDJSRKaCyohUdykDz4yIxI1jkqSMxdtiSyQwCaFuekjxJmkmVQOQ/3muNWw5HSMT6W4ctj8SgGudn8Agc+y80n6Pcb6XA07m5p5qR7kPV/7Csz3p7h2/aFVVBZnFNgALkkoosANTqJYvoxrmk+IwtQFKmZGVGuGJynOMvCyhT4zoRFrQz+k9MmKpVOdNde1Hb/2E0fae0Eoo9Wo1kT1iAWIuQBoNb3I85k/T7bLV8Q1JkVBh3dFIJLNqLlj25QbAecnOieGfEbMxFLezvUCF79YlEIJY7+vx7I0JoqHTHaNLEYp6tHNkZUBzDKSyoFJtysBLH0a6Z4iti6NJygpsCmVVtc5DlYsbknMo421MVwH0ZmwNfEAc1prf/vb/wBZadk9DsLQZXSmWdTcO7FiCNxA0UHtAiVjbRQel/RKvTxDvTR6qVXZ1KIzFSxLFGVQbWvodxEYYLodjHKj0DIpNsz2UKL7yGIOnK021zE981iZyEdl4NKNNKSCyooUc9OJ7SbnxlRxX0dUnd3NeoM7s9gqWGdi1h5y8gTgxtGU2UT/APmtH/76vknykzU6G0Gw1PDM9QpTdnVgyByzFib9W1useEsSiKARUPJlQwP0f4em+dKlYkK6gMUI66MhvZATox4ys7T+jWut/RVEqDX1ro3tuPbNWEBioFJlN+kzDk4OmQLlKgUczdDu/pjvEdH/APicLUzoowwpoQxsXHocgyniwKHSWxqKuMrqrDQ2YAi41BseUzD6WkdaqkZvRvQUHflLo9QjsJAcd2btmX2bRp14IhTOg7h7oIAZZsRwcNjaZ+vh86ntpkPb3n+UxXolhS1WkWFwjUFPHejEi/jaROw6vVrI4/5LAcDrfKfNx4Sz9FUyKWINms403ZHR/wCz3Ccy7Lv2aLg75FB9ZVKtfeSLa+Oh8ZD198mnAVi3CxVu6+h8Lnz7JCOdZrk8GeLydYalmcchqfDdJMxpgB63h8Y7M3xR1Znll+qMn+kXFZMfTekStSnTQkkaZrsVIvvFjbwifR/DV6u0hXphnUVRUdydFSoM1ix/A1gsvHSLommLr0qrsVVEKuqjrOM2ZRm+qNW7ddLb5O4egiKqIoRFFlVRYACWUSbkQ56J4Y4ipiHXO7tms+qKbAGyj1r2v1ryZZQLAAADcBoB4RRjEwJroxdhqJ2NIBE2eFBZy5naLOEEWjAJjE4bGEIgOliiTgRRRASAZ0qazlpDdLdrvQoKKdw9TMocfUVbZiPxdYW5TEpUbjG2Waims42vs2nWptTqorqw1Vhp3jiD2iZJh8ZjBvxVdbi9jWAuCN+plhGKxTf6V/SVD6N0p1OvcNkrA3fmSjqpPGxkXLZZRLhaCFeCbJmf7R6O5cSoRgpdMgUA6XCID5l3twC9olux2ACjKosAAe9Xpmk3fYKp8ZkKbWxHpb+nq3vv9I9/XPG8d4vbWJuP+Jrcf+a/4e2TN2bQj5qQb7SA/wBSj5yIK6kTLMNtrE5FH+prWyLp6V7bhwvEG2xiPvFb81/nMzdm+PRs2CTqk8z7ouTMYp7axNv/AJNb81/nD/bWJ+8VvzX+cvCVR6JTVs2UmFaY3+2sT94rfmv84DtrE/ea35r/ADm8/hjD6bJOgJjI21ifvNb81/nDO2sT94rfmv8AOLP4PH6bE7ROY4dtYn7xW/Nf5wDbWJ+8VvzX+cM/gsPptCLDYzGhtrE/ea35r/Oc/trE/eK35r/OGfwMPpscCzG/21ifvFb81/nDG2sT94rfmv8AOGfweP02dRFJi/7axP3it+a/znX7bxP3mt+a/wA4Z/BUbKZBdLaYNNG+yxX+oqf/AAmbftrE/eK35r/ONcftauyANXqkXO+o5+qeZmJPRSMaZvHRoWwFHsw6j+lLfCQexUth3Xga2b+l8Ow9gaZLs/buKAVRia4XKwy+lqZbXbS17RF9sYgU9MRWHX4VXH1V7Zzljc4JjH7axP3it+a/zglsiNH/2Q==</t>
   </si>
   <si>
-    <t>inter</t>
-  </si>
-  <si>
-    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcT3-m_3j1EZDCj4XI1iSeCIZP6xxWtO0NJlIdbyjzA&amp;s</t>
-  </si>
-  <si>
-    <t>cc</t>
-  </si>
-  <si>
-    <t>vn</t>
+    <t>Inter</t>
+  </si>
+  <si>
+    <t>https://itviec.com/rails/active_storage/representations/proxy/eyJfcmFpbHMiOnsibWVzc2FnZSI6IkJBaHBBNGsyREE9PSIsImV4cCI6bnVsbCwicHVyIjoiYmxvYl9pZCJ9fQ==--54a20447090fbe5c3893559090121b4b338e6596/eyJfcmFpbHMiOnsibWVzc2FnZSI6IkJBaDdCem9MWm05eWJXRjBTU0lJY0c1bkJqb0dSVlE2RW5KbGMybDZaVjkwYjE5bWFYUmJCMmtCcWpBPSIsImV4cCI6bnVsbCwicHVyIjoidmFyaWF0aW9uIn19--79eee5883893a012786006950460867831e6f661/nccsoft-logo.png</t>
+  </si>
+  <si>
+    <t>We do it with passion</t>
+  </si>
+  <si>
+    <t>138, Hà Huy Tập, Vinh, Nghệ An, Việt Nam</t>
   </si>
   <si>
     <t>play</t>
   </si>
   <si>
-    <t>ncc.com</t>
-  </si>
-  <si>
-    <t>the</t>
+    <t>http://ncc.asia/</t>
+  </si>
+  <si>
+    <t>the.letien</t>
+  </si>
+  <si>
+    <t>Lê Tiến Thế</t>
   </si>
   <si>
     <t>the.letien@ncc.asia</t>
@@ -99,10 +105,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -121,8 +127,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -150,18 +157,72 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -173,70 +234,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -244,6 +243,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -251,7 +257,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -266,187 +272,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -457,17 +463,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -527,6 +522,26 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
@@ -548,170 +563,164 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1035,13 +1044,22 @@
   <sheetPr/>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="2"/>
   <cols>
+    <col min="1" max="1" width="29.6363636363636" customWidth="1"/>
+    <col min="2" max="2" width="23.7272727272727" customWidth="1"/>
     <col min="3" max="3" width="20.6363636363636" customWidth="1"/>
+    <col min="5" max="5" width="24.3818181818182" customWidth="1"/>
+    <col min="6" max="6" width="13.0454545454545" customWidth="1"/>
+    <col min="7" max="7" width="13.0363636363636" customWidth="1"/>
+    <col min="8" max="8" width="15.5" customWidth="1"/>
+    <col min="9" max="9" width="27.5454545454545" customWidth="1"/>
+    <col min="10" max="10" width="47.8" customWidth="1"/>
+    <col min="12" max="12" width="17.9636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1083,86 +1101,89 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2">
         <v>113</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="H2" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" t="s">
         <v>21</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D3">
         <v>114</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
         <v>17</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" t="s">
-        <v>21</v>
+        <v>27</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="dat.lethanh2@ncc.asia"/>
     <hyperlink ref="C3" r:id="rId2" display="the.letien@ncc.asia"/>
-    <hyperlink ref="H2" r:id="rId3" display="https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcT3-m_3j1EZDCj4XI1iSeCIZP6xxWtO0NJlIdbyjzA&amp;s"/>
+    <hyperlink ref="H2" r:id="rId3" display="https://itviec.com/rails/active_storage/representations/proxy/eyJfcmFpbHMiOnsibWVzc2FnZSI6IkJBaHBBNGsyREE9PSIsImV4cCI6bnVsbCwicHVyIjoiYmxvYl9pZCJ9fQ==--54a20447090fbe5c3893559090121b4b338e6596/eyJfcmFpbHMiOnsibWVzc2FnZSI6IkJBaDdCem9MWm05eWJXRjBTU0lJY0c1bkJqb0dSVlE2RW5KbGMybDZaVjkwYjE5bWFYUmJCMmtCcWpBPSIsImV4cCI6bnVsbCwicHVyIjoidmFyaWF0aW9uIn19--79eee5883893a012786006950460867831e6f661/nccsoft-logo.png" tooltip="https://itviec.com/rails/active_storage/representations/proxy/eyJfcmFpbHMiOnsibWVzc2FnZSI6IkJBaHBBNGsyREE9PSIsImV4cCI6bnVsbCwicHVyIjoiYmxvYl9pZCJ9fQ==--54a20447090fbe5c3893559090121b4b338e6596/eyJfcmFpbHMiOnsibWVzc2FnZSI6IkJBaDdCem9MWm05eWJXRjBTU0lJY0c1bk"/>
+    <hyperlink ref="H3" r:id="rId3" display="https://itviec.com/rails/active_storage/representations/proxy/eyJfcmFpbHMiOnsibWVzc2FnZSI6IkJBaHBBNGsyREE9PSIsImV4cCI6bnVsbCwicHVyIjoiYmxvYl9pZCJ9fQ==--54a20447090fbe5c3893559090121b4b338e6596/eyJfcmFpbHMiOnsibWVzc2FnZSI6IkJBaDdCem9MWm05eWJXRjBTU0lJY0c1bkJqb0dSVlE2RW5KbGMybDZaVjkwYjE5bWFYUmJCMmtCcWpBPSIsImV4cCI6bnVsbCwicHVyIjoidmFyaWF0aW9uIn19--79eee5883893a012786006950460867831e6f661/nccsoft-logo.png"/>
+    <hyperlink ref="L2" r:id="rId4" display="http://ncc.asia/"/>
+    <hyperlink ref="L3" r:id="rId4" display="http://ncc.asia/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>